<commit_message>
Add status checking after update attempt
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0C1EC7-8455-43C1-A67F-4068E60EAAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C8C6E-A3AE-4660-8ACD-1CC272E5B3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
+    <workbookView xWindow="28680" yWindow="-4755" windowWidth="16440" windowHeight="28440" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Release Definition Name</t>
+    <t>Release Name</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add status monitoring after update (#3)
- Add constants files
- Add status  monitoring method to utile
- Impalement update status monitoring in update script
- Change excel file headers
- Add handling of already in-progress release status
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0C1EC7-8455-43C1-A67F-4068E60EAAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C8C6E-A3AE-4660-8ACD-1CC272E5B3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
+    <workbookView xWindow="28680" yWindow="-4755" windowWidth="16440" windowHeight="28440" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Release Definition Name</t>
+    <t>Release Name</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implement critical release update handling
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C8C6E-A3AE-4660-8ACD-1CC272E5B3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA72864-E961-4EA6-8518-813FC5D1B20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4755" windowWidth="16440" windowHeight="28440" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
+    <workbookView xWindow="28800" yWindow="-4635" windowWidth="16200" windowHeight="8055" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Release Number</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Release Name</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -402,19 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F26F02E-433B-4821-A488-863521E826B7}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="20.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -427,6 +432,9 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement critical release update handling (#4)
Add critical header to excel file
Include critical in release-to-update object
Add method for handling failed updates
Implement critical update handling in update failed method
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690C8C6E-A3AE-4660-8ACD-1CC272E5B3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA72864-E961-4EA6-8518-813FC5D1B20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4755" windowWidth="16440" windowHeight="28440" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
+    <workbookView xWindow="28800" yWindow="-4635" windowWidth="16200" windowHeight="8055" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Release Number</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Release Name</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
@@ -402,19 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F26F02E-433B-4821-A488-863521E826B7}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="20.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -427,6 +432,9 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change instances of "critical" to "is_crucial"
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA72864-E961-4EA6-8518-813FC5D1B20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642C134-52BA-4F36-BB21-D8DCA79049EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-4635" windowWidth="16200" windowHeight="8055" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Release Name</t>
   </si>
   <si>
-    <t>Critical</t>
+    <t>Crucial</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change instances of "critical" to "is_crucial" (#5)
</commit_message>
<xml_diff>
--- a/files/deployment-plan.xlsx
+++ b/files/deployment-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Fun\Python\ado-auto-delivery\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA72864-E961-4EA6-8518-813FC5D1B20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642C134-52BA-4F36-BB21-D8DCA79049EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-4635" windowWidth="16200" windowHeight="8055" xr2:uid="{6B967F0F-6D7C-430B-BC59-0230DFF1D9B1}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Release Name</t>
   </si>
   <si>
-    <t>Critical</t>
+    <t>Crucial</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>